<commit_message>
Chnages to SCoP count chart
</commit_message>
<xml_diff>
--- a/tests/polybench-c-4.0/results/final-charts-2.xlsx
+++ b/tests/polybench-c-4.0/results/final-charts-2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="0" windowWidth="24080" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1160" yWindow="0" windowWidth="31480" windowHeight="21080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="code-size" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="40">
   <si>
     <t>benchmark</t>
   </si>
@@ -137,20 +137,17 @@
     <t>SCEV and ISL compilation time (seconds)</t>
   </si>
   <si>
-    <t>SCEV and ISL number of SCoPs</t>
+    <t>PDA</t>
   </si>
   <si>
-    <t>floyd-warshall</t>
-  </si>
-  <si>
-    <t>PDA</t>
+    <t>Number of SCoPs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,6 +199,12 @@
       <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -330,7 +333,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -520,8 +523,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -561,6 +574,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -570,22 +593,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -680,6 +704,11 @@
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -774,6 +803,11 @@
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1262,11 +1296,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2083701528"/>
-        <c:axId val="2083698472"/>
+        <c:axId val="-2130349544"/>
+        <c:axId val="-2130346520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2083701528"/>
+        <c:axId val="-2130349544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,7 +1310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="2083698472"/>
+        <c:crossAx val="-2130346520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1284,7 +1318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083698472"/>
+        <c:axId val="-2130346520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1318,7 +1352,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083701528"/>
+        <c:crossAx val="-2130349544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -1841,11 +1875,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2083620472"/>
-        <c:axId val="2083617416"/>
+        <c:axId val="-2130270872"/>
+        <c:axId val="-2130267848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2083620472"/>
+        <c:axId val="-2130270872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1855,7 +1889,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="2083617416"/>
+        <c:crossAx val="-2130267848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1863,7 +1897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083617416"/>
+        <c:axId val="-2130267848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60.0"/>
@@ -1916,7 +1950,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083620472"/>
+        <c:crossAx val="-2130270872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1981,7 +2015,7 @@
           <c:x val="0.0601813153535112"/>
           <c:y val="0.0831182560513269"/>
           <c:w val="0.930912319646887"/>
-          <c:h val="0.664245042286381"/>
+          <c:h val="0.631095836777309"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1993,7 +2027,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'#-of-scops'!$A$4</c:f>
+              <c:f>'#-of-scops'!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2019,92 +2053,92 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'#-of-scops'!$A$6:$A$34</c:f>
+              <c:f>'#-of-scops'!$B$6:$B$34</c:f>
               <c:strCache>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>gemm</c:v>
+                  <c:v>nussinov</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>seidel-2d</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>symm</c:v>
+                  <c:v>atax</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>atax</c:v>
+                  <c:v>durbin</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>doitgen</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>gemm</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>adi</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>durbin</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>heat-3d</c:v>
+                  <c:v>bicg</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>ludcmp</c:v>
+                  <c:v>syrk</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>3mm</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>bicg</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>cholesky</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>gemver</c:v>
+                  <c:v>syr2k</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>syrk</c:v>
+                  <c:v>trmm</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2mm</c:v>
+                  <c:v>fdtd-2d</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>trisolv</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>gramschmidt</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>symm</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>correlation</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>fdtd-2d</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>syr2k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>trisolv</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>mvt</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>covariance</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>ludcmp</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>mvt</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>gesummv</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>heat-3d</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>jacobi-2d</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>gramschmidt</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
+                  <c:v>gemver</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>jacobi-1d</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>lu</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>trmm</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>nussinov</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>gesummv</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>deriche</c:v>
@@ -2114,18 +2148,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'#-of-scops'!$D$6:$D$34</c:f>
+              <c:f>'#-of-scops'!$E$6:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>1.4</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.333333333333333</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.25</c:v>
@@ -2134,46 +2168,46 @@
                   <c:v>1.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.25</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5</c:v>
+                  <c:v>1.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5</c:v>
+                  <c:v>1.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.6</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.666666666666667</c:v>
+                  <c:v>2.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0</c:v>
+                  <c:v>2.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2.5</c:v>
@@ -2182,25 +2216,25 @@
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.333333333333333</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>4.5</c:v>
@@ -2214,7 +2248,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'#-of-scops'!$F$4</c:f>
+              <c:f>'#-of-scops'!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2239,92 +2273,92 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'#-of-scops'!$A$6:$A$34</c:f>
+              <c:f>'#-of-scops'!$B$6:$B$34</c:f>
               <c:strCache>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>gemm</c:v>
+                  <c:v>nussinov</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>seidel-2d</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>symm</c:v>
+                  <c:v>atax</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>atax</c:v>
+                  <c:v>durbin</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>doitgen</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>gemm</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>adi</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>durbin</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>heat-3d</c:v>
+                  <c:v>bicg</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>ludcmp</c:v>
+                  <c:v>syrk</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>3mm</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>bicg</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>cholesky</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>gemver</c:v>
+                  <c:v>syr2k</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>syrk</c:v>
+                  <c:v>trmm</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2mm</c:v>
+                  <c:v>fdtd-2d</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>trisolv</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>gramschmidt</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>symm</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>correlation</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>fdtd-2d</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>syr2k</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>trisolv</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>mvt</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>covariance</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>ludcmp</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>mvt</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>gesummv</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>heat-3d</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>jacobi-2d</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>gramschmidt</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
+                  <c:v>gemver</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>jacobi-1d</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>lu</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>trmm</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>nussinov</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>gesummv</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>deriche</c:v>
@@ -2334,18 +2368,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'#-of-scops'!$I$6:$I$34</c:f>
+              <c:f>'#-of-scops'!$J$6:$J$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.75</c:v>
@@ -2354,73 +2388,73 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.25</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.75</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.6</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0</c:v>
+                  <c:v>1.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2.0</c:v>
@@ -2434,7 +2468,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'#-of-scops'!$K$4:$N$4</c:f>
+              <c:f>'#-of-scops'!$L$4:$O$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2458,96 +2492,96 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'#-of-scops'!$N$6:$N$34</c:f>
+              <c:f>'#-of-scops'!$O$6:$O$34</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.75</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="25">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>16.0</c:v>
-                </c:pt>
                 <c:pt idx="28">
-                  <c:v>22.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2562,11 +2596,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2067077800"/>
-        <c:axId val="2067074744"/>
+        <c:axId val="-2130214184"/>
+        <c:axId val="-2130211176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2067077800"/>
+        <c:axId val="-2130214184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2576,7 +2610,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="2067074744"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2130211176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2584,7 +2628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2067074744"/>
+        <c:axId val="-2130211176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2608,10 +2652,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Ratio</a:t>
                 </a:r>
               </a:p>
@@ -2631,12 +2675,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1200"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2067077800"/>
+        <c:crossAx val="-2130214184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2647,10 +2691,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.433238401842406"/>
-          <c:y val="0.0974700445053064"/>
-          <c:w val="0.0782538498341672"/>
-          <c:h val="0.374215777375654"/>
+          <c:x val="0.435303626080197"/>
+          <c:y val="0.108618404304813"/>
+          <c:w val="0.0956838255898468"/>
+          <c:h val="0.279455578086184"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2664,6 +2708,16 @@
           </a:solidFill>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -2753,16 +2807,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>27940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3122,50 +3176,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="4" spans="1:13" ht="16" thickBot="1">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="G4" s="21" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="G4" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:13" ht="16" thickBot="1">
       <c r="A5" s="1" t="s">
@@ -4409,50 +4463,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="4" spans="1:13" ht="16" thickBot="1">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="G4" s="21" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="G4" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:13" ht="16" thickBot="1">
       <c r="A5" s="1" t="s">
@@ -5682,1377 +5736,1394 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N67"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="2.1640625" customWidth="1"/>
-    <col min="6" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="2.1640625" customWidth="1"/>
-    <col min="11" max="18" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="4" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="2.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="9" width="7.83203125" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="2.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="14" width="7.83203125" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
+    <col min="16" max="17" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="2:15" ht="15" customHeight="1">
+      <c r="B1" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+    </row>
+    <row r="2" spans="2:15" ht="15" customHeight="1">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+    </row>
+    <row r="4" spans="2:15" ht="16" thickBot="1">
+      <c r="B4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="G4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+      <c r="L4" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-    </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1">
-      <c r="A4" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="F4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="K4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-    </row>
-    <row r="5" spans="1:14" ht="16" thickBot="1">
-      <c r="A5" s="1" t="s">
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+    </row>
+    <row r="5" spans="2:15" ht="16" thickBot="1">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="D5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="E5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="J5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="L5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="M5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="26" t="s">
+      <c r="N5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="27" t="s">
+      <c r="O5" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
+    <row r="6" spans="2:15">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="28">
+        <v>3</v>
+      </c>
+      <c r="D6" s="29">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" ref="E6:E34" si="0">D6/C6</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="28">
+        <v>4</v>
+      </c>
+      <c r="I6" s="30">
+        <v>3</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" ref="J6:J34" si="1">I6/H6</f>
+        <v>0.75</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="31">
+        <v>3</v>
+      </c>
+      <c r="N6" s="32">
+        <v>2</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" ref="O6:O34" si="2">N6/M6</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="28">
+        <v>3</v>
+      </c>
+      <c r="D7" s="29">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="28">
+        <v>3</v>
+      </c>
+      <c r="I7" s="30">
+        <v>3</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="28">
+        <v>3</v>
+      </c>
+      <c r="N7" s="29">
+        <v>2</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="28">
+        <v>4</v>
+      </c>
+      <c r="D8" s="29">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="28">
+        <v>4</v>
+      </c>
+      <c r="I8" s="30">
+        <v>3</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="28">
+        <v>4</v>
+      </c>
+      <c r="N8" s="29">
+        <v>4</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="28">
+        <v>4</v>
+      </c>
+      <c r="D9" s="29">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="28">
+        <v>4</v>
+      </c>
+      <c r="I9" s="30">
+        <v>3</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="28">
+        <v>4</v>
+      </c>
+      <c r="N9" s="29">
+        <v>5</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="28">
+        <v>3</v>
+      </c>
+      <c r="D10" s="29">
+        <v>4</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="28">
+        <v>3</v>
+      </c>
+      <c r="I10" s="30">
+        <v>3</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="28">
+        <v>3</v>
+      </c>
+      <c r="N10" s="29">
+        <v>3</v>
+      </c>
+      <c r="O10" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="5">
+      <c r="C11" s="28">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="D11" s="29">
         <v>7</v>
       </c>
-      <c r="D6" s="7">
-        <f>C6/B6</f>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H11" s="28">
         <v>5</v>
       </c>
-      <c r="H6" s="30">
+      <c r="I11" s="30">
         <v>3</v>
       </c>
-      <c r="I6" s="7">
-        <f>H6/G6</f>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="K6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="28">
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="28">
+        <v>5</v>
+      </c>
+      <c r="N11" s="29">
         <v>6</v>
       </c>
-      <c r="M6" s="29">
+      <c r="O11" s="13">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="28">
+        <v>2</v>
+      </c>
+      <c r="D12" s="29">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="28">
+        <v>2</v>
+      </c>
+      <c r="I12" s="30">
+        <v>3</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="28">
+        <v>2</v>
+      </c>
+      <c r="N12" s="29">
+        <v>2</v>
+      </c>
+      <c r="O12" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="28">
+        <v>4</v>
+      </c>
+      <c r="D13" s="29">
         <v>6</v>
       </c>
-      <c r="N6">
-        <f>M6/L6</f>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="28">
+        <v>4</v>
+      </c>
+      <c r="I13" s="30">
+        <v>3</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" s="28">
+        <v>4</v>
+      </c>
+      <c r="N13" s="29">
+        <v>4</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
+    <row r="14" spans="2:15">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="28">
+        <v>4</v>
+      </c>
+      <c r="D14" s="29">
+        <v>6</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="28">
+        <v>4</v>
+      </c>
+      <c r="I14" s="30">
+        <v>3</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="28">
+        <v>4</v>
+      </c>
+      <c r="N14" s="29">
+        <v>5</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="28">
+        <v>5</v>
+      </c>
+      <c r="D15" s="29">
+        <v>8</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="28">
+        <v>5</v>
+      </c>
+      <c r="I15" s="30">
+        <v>3</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="L15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="28">
+        <v>5</v>
+      </c>
+      <c r="N15" s="29">
+        <v>5</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="28">
+        <v>5</v>
+      </c>
+      <c r="D16" s="29">
+        <v>8</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="28">
+        <v>5</v>
+      </c>
+      <c r="I16" s="30">
+        <v>3</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="L16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="28">
+        <v>5</v>
+      </c>
+      <c r="N16" s="29">
+        <v>4</v>
+      </c>
+      <c r="O16" s="13">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="28">
+        <v>6</v>
+      </c>
+      <c r="D17" s="29">
+        <v>10</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="28">
+        <v>5</v>
+      </c>
+      <c r="I17" s="30">
+        <v>6</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="28">
+        <v>6</v>
+      </c>
+      <c r="N17" s="29">
+        <v>7</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="2"/>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="28">
+        <v>3</v>
+      </c>
+      <c r="D18" s="29">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="28">
+        <v>3</v>
+      </c>
+      <c r="I18" s="30">
+        <v>3</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M18" s="28">
+        <v>3</v>
+      </c>
+      <c r="N18" s="29">
+        <v>4</v>
+      </c>
+      <c r="O18" s="13">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="28">
+        <v>3</v>
+      </c>
+      <c r="D19" s="29">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="28">
+        <v>3</v>
+      </c>
+      <c r="I19" s="30">
+        <v>3</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="28">
+        <v>3</v>
+      </c>
+      <c r="N19" s="29">
+        <v>4</v>
+      </c>
+      <c r="O19" s="13">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="28">
+        <v>2</v>
+      </c>
+      <c r="D20" s="29">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="28">
+        <v>2</v>
+      </c>
+      <c r="I20" s="30">
+        <v>3</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="L20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="28">
+        <v>2</v>
+      </c>
+      <c r="N20" s="29">
+        <v>3</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="28">
+        <v>6</v>
+      </c>
+      <c r="D21" s="29">
+        <v>12</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="28">
+        <v>4</v>
+      </c>
+      <c r="I21" s="30">
+        <v>5</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="L21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="28">
+        <v>6</v>
+      </c>
+      <c r="N21" s="29">
+        <v>7</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" si="2"/>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="28">
+        <v>2</v>
+      </c>
+      <c r="D22" s="29">
+        <v>4</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="28">
+        <v>2</v>
+      </c>
+      <c r="I22" s="30">
+        <v>3</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="28">
+        <v>2</v>
+      </c>
+      <c r="N22" s="29">
+        <v>3</v>
+      </c>
+      <c r="O22" s="13">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="28">
+        <v>3</v>
+      </c>
+      <c r="D23" s="29">
+        <v>7</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="28">
+        <v>3</v>
+      </c>
+      <c r="I23" s="30">
+        <v>5</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="28">
+        <v>3</v>
+      </c>
+      <c r="N23" s="29">
+        <v>2</v>
+      </c>
+      <c r="O23" s="13">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="28">
+        <v>3</v>
+      </c>
+      <c r="D24" s="29">
+        <v>7</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="28">
+        <v>2</v>
+      </c>
+      <c r="I24" s="30">
+        <v>3</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="L24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="28">
+        <v>3</v>
+      </c>
+      <c r="N24" s="29">
+        <v>3</v>
+      </c>
+      <c r="O24" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="28">
+        <v>2</v>
+      </c>
+      <c r="D25" s="29">
+        <v>5</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="28">
+        <v>2</v>
+      </c>
+      <c r="I25" s="29">
+        <v>5</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="L25" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" s="28">
+        <v>2</v>
+      </c>
+      <c r="N25" s="29">
+        <v>1</v>
+      </c>
+      <c r="O25" s="13">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="28">
+        <v>2</v>
+      </c>
+      <c r="D26" s="29">
+        <v>5</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="28">
+        <v>2</v>
+      </c>
+      <c r="I26" s="30">
+        <v>3</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="L26" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="28">
+        <v>2</v>
+      </c>
+      <c r="N26" s="29">
+        <v>2</v>
+      </c>
+      <c r="O26" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="28">
+        <v>6</v>
+      </c>
+      <c r="D27" s="29">
         <v>15</v>
       </c>
-      <c r="B7" s="5">
+      <c r="E27" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="28">
+        <v>4</v>
+      </c>
+      <c r="I27" s="30">
+        <v>5</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="L27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="28">
+        <v>6</v>
+      </c>
+      <c r="N27" s="29">
+        <v>6</v>
+      </c>
+      <c r="O27" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="29">
+        <v>5</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="28">
+        <v>2</v>
+      </c>
+      <c r="I28" s="30">
         <v>3</v>
       </c>
-      <c r="C7" s="6">
+      <c r="J28" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="L28" t="s">
+        <v>26</v>
+      </c>
+      <c r="M28" s="28">
+        <v>2</v>
+      </c>
+      <c r="N28" s="29">
+        <v>2</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="28">
+        <v>1</v>
+      </c>
+      <c r="D29" s="29">
         <v>3</v>
       </c>
-      <c r="D7" s="7">
-        <f>C7/B7</f>
+      <c r="E29" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="28">
         <v>1</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="I29" s="30">
         <v>3</v>
       </c>
-      <c r="H7" s="30">
+      <c r="J29" s="7">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I7" s="7">
-        <f>H7/G7</f>
+      <c r="L29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" s="28">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="28">
+      <c r="N29" s="29">
+        <v>1</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="29">
+      <c r="C30" s="28">
+        <v>1</v>
+      </c>
+      <c r="D30" s="29">
+        <v>3</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" t="s">
         <v>6</v>
       </c>
-      <c r="N7">
-        <f>M7/L7</f>
+      <c r="H30" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="I30" s="30">
         <v>3</v>
       </c>
-      <c r="C8" s="6">
+      <c r="J30" s="7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M30" s="28">
+        <v>1</v>
+      </c>
+      <c r="N30" s="29">
+        <v>2</v>
+      </c>
+      <c r="O30" s="13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="28">
+        <v>1</v>
+      </c>
+      <c r="D31" s="29">
+        <v>3</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="28">
+        <v>1</v>
+      </c>
+      <c r="I31" s="30">
+        <v>3</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L31" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" s="28">
+        <v>1</v>
+      </c>
+      <c r="N31" s="29">
+        <v>2</v>
+      </c>
+      <c r="O31" s="13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="28">
+        <v>2</v>
+      </c>
+      <c r="D32" s="29">
         <v>7</v>
       </c>
-      <c r="D8" s="7">
-        <f>C8/B8</f>
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="E32" s="7">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="28">
         <v>2</v>
       </c>
-      <c r="H8" s="30">
+      <c r="I32" s="30">
         <v>3</v>
       </c>
-      <c r="I8" s="7">
-        <f>H8/G8</f>
+      <c r="J32" s="7">
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="28">
-        <v>6</v>
-      </c>
-      <c r="M8" s="29">
-        <v>6</v>
-      </c>
-      <c r="N8">
-        <f>M8/L8</f>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" s="28">
+        <v>2</v>
+      </c>
+      <c r="N32" s="29">
+        <v>4</v>
+      </c>
+      <c r="O32" s="13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="D33" s="29">
         <v>4</v>
       </c>
-      <c r="C9" s="6">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7">
-        <f>C9/B9</f>
-        <v>1.25</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="E33" s="7">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H9" s="30">
+      <c r="F33" s="13"/>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="28">
+        <v>1</v>
+      </c>
+      <c r="I33" s="30">
+        <v>4</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L33" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="28">
+        <v>1</v>
+      </c>
+      <c r="N33" s="29">
         <v>3</v>
       </c>
-      <c r="I9" s="7">
-        <f>H9/G9</f>
-        <v>0.75</v>
-      </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="28">
-        <v>8</v>
-      </c>
-      <c r="M9" s="29">
-        <v>14</v>
-      </c>
-      <c r="N9">
-        <f>M9/L9</f>
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5">
+      <c r="O33" s="13">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="C10" s="6">
+    </row>
+    <row r="34" spans="2:15">
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="28">
+        <v>2</v>
+      </c>
+      <c r="D34" s="29">
+        <v>9</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="28">
+        <v>2</v>
+      </c>
+      <c r="I34" s="30">
         <v>4</v>
       </c>
-      <c r="D10" s="7">
-        <f>C10/B10</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="5">
-        <v>3</v>
-      </c>
-      <c r="H10" s="30">
-        <v>3</v>
-      </c>
-      <c r="I10" s="7">
-        <f>H10/G10</f>
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" s="28">
-        <v>6</v>
-      </c>
-      <c r="M10" s="29">
-        <v>12</v>
-      </c>
-      <c r="N10">
-        <f>M10/L10</f>
+      <c r="J34" s="7">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5">
+      <c r="L34" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" s="28">
         <v>2</v>
       </c>
-      <c r="C11" s="6">
-        <v>3</v>
-      </c>
-      <c r="D11" s="7">
-        <f>C11/B11</f>
-        <v>1.5</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="N34" s="29">
+        <v>4</v>
+      </c>
+      <c r="O34" s="13">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H11" s="30">
-        <v>3</v>
-      </c>
-      <c r="I11" s="7">
-        <f>H11/G11</f>
-        <v>1.5</v>
-      </c>
-      <c r="K11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="28">
-        <v>4</v>
-      </c>
-      <c r="M11" s="29">
-        <v>10</v>
-      </c>
-      <c r="N11">
-        <f>M11/L11</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5">
-        <v>4</v>
-      </c>
-      <c r="C12" s="6">
-        <v>5</v>
-      </c>
-      <c r="D12" s="7">
-        <f>C12/B12</f>
-        <v>1.25</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="5">
-        <v>4</v>
-      </c>
-      <c r="H12" s="30">
-        <v>3</v>
-      </c>
-      <c r="I12" s="7">
-        <f>H12/G12</f>
-        <v>0.75</v>
-      </c>
-      <c r="K12" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" s="28">
-        <v>4</v>
-      </c>
-      <c r="M12" s="29">
-        <v>10</v>
-      </c>
-      <c r="N12">
-        <f>M12/L12</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6">
-        <v>3</v>
-      </c>
-      <c r="D13" s="7">
-        <f>C13/B13</f>
-        <v>3</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
-      </c>
-      <c r="H13" s="30">
-        <v>3</v>
-      </c>
-      <c r="I13" s="7">
-        <f>H13/G13</f>
-        <v>3</v>
-      </c>
-      <c r="K13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="28">
-        <v>4</v>
-      </c>
-      <c r="M13" s="29">
-        <v>10</v>
-      </c>
-      <c r="N13">
-        <f>M13/L13</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="5">
-        <v>6</v>
-      </c>
-      <c r="C14" s="6">
-        <v>15</v>
-      </c>
-      <c r="D14" s="7">
-        <f>C14/B14</f>
-        <v>2.5</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="5">
-        <v>4</v>
-      </c>
-      <c r="H14" s="30">
-        <v>5</v>
-      </c>
-      <c r="I14" s="7">
-        <f>H14/G14</f>
-        <v>1.25</v>
-      </c>
-      <c r="K14" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="28">
-        <v>8</v>
-      </c>
-      <c r="M14" s="29">
-        <v>20</v>
-      </c>
-      <c r="N14">
-        <f>M14/L14</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="5">
-        <v>5</v>
-      </c>
-      <c r="C15" s="6">
-        <v>8</v>
-      </c>
-      <c r="D15" s="7">
-        <f>C15/B15</f>
-        <v>1.6</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="5">
-        <v>5</v>
-      </c>
-      <c r="H15" s="30">
-        <v>3</v>
-      </c>
-      <c r="I15" s="7">
-        <f>H15/G15</f>
-        <v>0.6</v>
-      </c>
-      <c r="K15" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="28">
-        <v>10</v>
-      </c>
-      <c r="M15" s="29">
-        <v>28</v>
-      </c>
-      <c r="N15">
-        <f>M15/L15</f>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="5">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6">
-        <v>6</v>
-      </c>
-      <c r="D16" s="7">
-        <f>C16/B16</f>
-        <v>1.5</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="5">
-        <v>4</v>
-      </c>
-      <c r="H16" s="30">
-        <v>3</v>
-      </c>
-      <c r="I16" s="7">
-        <f>H16/G16</f>
-        <v>0.75</v>
-      </c>
-      <c r="K16" t="s">
-        <v>32</v>
-      </c>
-      <c r="L16" s="28">
-        <v>6</v>
-      </c>
-      <c r="M16" s="29">
-        <v>18</v>
-      </c>
-      <c r="N16">
-        <f>M16/L16</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="5">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6">
-        <v>10</v>
-      </c>
-      <c r="D17" s="7">
-        <f>C17/B17</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="5">
-        <v>5</v>
-      </c>
-      <c r="H17" s="30">
-        <v>6</v>
-      </c>
-      <c r="I17" s="7">
-        <f>H17/G17</f>
-        <v>1.2</v>
-      </c>
-      <c r="K17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="28">
-        <v>6</v>
-      </c>
-      <c r="M17" s="29">
-        <v>18</v>
-      </c>
-      <c r="N17">
-        <f>M17/L17</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="5">
-        <v>2</v>
-      </c>
-      <c r="C18" s="6">
-        <v>7</v>
-      </c>
-      <c r="D18" s="7">
-        <f>C18/B18</f>
-        <v>3.5</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="5">
-        <v>2</v>
-      </c>
-      <c r="H18" s="30">
-        <v>3</v>
-      </c>
-      <c r="I18" s="7">
-        <f>H18/G18</f>
-        <v>1.5</v>
-      </c>
-      <c r="K18" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" s="28">
-        <v>6</v>
-      </c>
-      <c r="M18" s="29">
-        <v>18</v>
-      </c>
-      <c r="N18">
-        <f>M18/L18</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="5">
-        <v>4</v>
-      </c>
-      <c r="C19" s="6">
-        <v>6</v>
-      </c>
-      <c r="D19" s="7">
-        <f>C19/B19</f>
-        <v>1.5</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="5">
-        <v>4</v>
-      </c>
-      <c r="H19" s="30">
-        <v>3</v>
-      </c>
-      <c r="I19" s="7">
-        <f>H19/G19</f>
-        <v>0.75</v>
-      </c>
-      <c r="K19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" s="28">
-        <v>6</v>
-      </c>
-      <c r="M19" s="29">
-        <v>18</v>
-      </c>
-      <c r="N19">
-        <f>M19/L19</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="5">
-        <v>5</v>
-      </c>
-      <c r="C20" s="6">
-        <v>8</v>
-      </c>
-      <c r="D20" s="7">
-        <f>C20/B20</f>
-        <v>1.6</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="5">
-        <v>5</v>
-      </c>
-      <c r="H20" s="30">
-        <v>3</v>
-      </c>
-      <c r="I20" s="7">
-        <f>H20/G20</f>
-        <v>0.6</v>
-      </c>
-      <c r="K20" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" s="28">
-        <v>8</v>
-      </c>
-      <c r="M20" s="29">
-        <v>26</v>
-      </c>
-      <c r="N20">
-        <f>M20/L20</f>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="5">
-        <v>2</v>
-      </c>
-      <c r="C21" s="6">
-        <v>5</v>
-      </c>
-      <c r="D21" s="7">
-        <f>C21/B21</f>
-        <v>2.5</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="5">
-        <v>2</v>
-      </c>
-      <c r="H21" s="6">
-        <v>5</v>
-      </c>
-      <c r="I21" s="7">
-        <f>H21/G21</f>
-        <v>2.5</v>
-      </c>
-      <c r="K21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21" s="28">
-        <v>4</v>
-      </c>
-      <c r="M21" s="29">
-        <v>16</v>
-      </c>
-      <c r="N21">
-        <f>M21/L21</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="5">
-        <v>2</v>
-      </c>
-      <c r="C22" s="6">
-        <v>4</v>
-      </c>
-      <c r="D22" s="7">
-        <f>C22/B22</f>
-        <v>2</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="5">
-        <v>2</v>
-      </c>
-      <c r="H22" s="30">
-        <v>3</v>
-      </c>
-      <c r="I22" s="7">
-        <f>H22/G22</f>
-        <v>1.5</v>
-      </c>
-      <c r="K22" t="s">
-        <v>10</v>
-      </c>
-      <c r="L22" s="28">
-        <v>4</v>
-      </c>
-      <c r="M22" s="29">
-        <v>16</v>
-      </c>
-      <c r="N22">
-        <f>M22/L22</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="5">
-        <v>3</v>
-      </c>
-      <c r="C23" s="6">
-        <v>5</v>
-      </c>
-      <c r="D23" s="7">
-        <f>C23/B23</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="5">
-        <v>3</v>
-      </c>
-      <c r="H23" s="30">
-        <v>3</v>
-      </c>
-      <c r="I23" s="7">
-        <f>H23/G23</f>
-        <v>1</v>
-      </c>
-      <c r="K23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="28">
-        <v>4</v>
-      </c>
-      <c r="M23" s="29">
-        <v>16</v>
-      </c>
-      <c r="N23">
-        <f>M23/L23</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="5">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6">
-        <v>4</v>
-      </c>
-      <c r="D24" s="7">
-        <f>C24/B24</f>
-        <v>2</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="5">
-        <v>2</v>
-      </c>
-      <c r="H24" s="30">
-        <v>3</v>
-      </c>
-      <c r="I24" s="7">
-        <f>H24/G24</f>
-        <v>1.5</v>
-      </c>
-      <c r="K24" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" s="28">
-        <v>4</v>
-      </c>
-      <c r="M24" s="29">
-        <v>16</v>
-      </c>
-      <c r="N24">
-        <f>M24/L24</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="5">
-        <v>2</v>
-      </c>
-      <c r="C25" s="6">
-        <v>5</v>
-      </c>
-      <c r="D25" s="7">
-        <f>C25/B25</f>
-        <v>2.5</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="5">
-        <v>2</v>
-      </c>
-      <c r="H25" s="30">
-        <v>3</v>
-      </c>
-      <c r="I25" s="7">
-        <f>H25/G25</f>
-        <v>1.5</v>
-      </c>
-      <c r="K25" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25" s="28">
-        <v>8</v>
-      </c>
-      <c r="M25" s="29">
-        <v>38</v>
-      </c>
-      <c r="N25">
-        <f>M25/L25</f>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="5">
-        <v>2</v>
-      </c>
-      <c r="C26" s="6">
-        <v>5</v>
-      </c>
-      <c r="D26" s="7">
-        <f>C26/B26</f>
-        <v>2.5</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="5">
-        <v>2</v>
-      </c>
-      <c r="H26" s="30">
-        <v>3</v>
-      </c>
-      <c r="I26" s="7">
-        <f>H26/G26</f>
-        <v>1.5</v>
-      </c>
-      <c r="K26" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="28">
-        <v>4</v>
-      </c>
-      <c r="M26" s="29">
-        <v>22</v>
-      </c>
-      <c r="N26">
-        <f>M26/L26</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6">
-        <v>3</v>
-      </c>
-      <c r="D27" s="7">
-        <f>C27/B27</f>
-        <v>3</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="5">
-        <v>1</v>
-      </c>
-      <c r="H27" s="30">
-        <v>3</v>
-      </c>
-      <c r="I27" s="7">
-        <f>H27/G27</f>
-        <v>3</v>
-      </c>
-      <c r="K27" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="28">
-        <v>2</v>
-      </c>
-      <c r="M27" s="29">
-        <v>12</v>
-      </c>
-      <c r="N27">
-        <f>M27/L27</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="5">
-        <v>3</v>
-      </c>
-      <c r="C28" s="6">
-        <v>7</v>
-      </c>
-      <c r="D28" s="7">
-        <f>C28/B28</f>
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="5">
-        <v>3</v>
-      </c>
-      <c r="H28" s="30">
-        <v>5</v>
-      </c>
-      <c r="I28" s="7">
-        <f>H28/G28</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="K28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L28" s="28">
-        <v>2</v>
-      </c>
-      <c r="M28" s="29">
-        <v>14</v>
-      </c>
-      <c r="N28">
-        <f>M28/L28</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-      <c r="C29" s="6">
-        <v>4</v>
-      </c>
-      <c r="D29" s="7">
-        <f>C29/B29</f>
-        <v>4</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1</v>
-      </c>
-      <c r="H29" s="30">
-        <v>4</v>
-      </c>
-      <c r="I29" s="7">
-        <f>H29/G29</f>
-        <v>4</v>
-      </c>
-      <c r="K29" t="s">
-        <v>6</v>
-      </c>
-      <c r="L29" s="28">
-        <v>2</v>
-      </c>
-      <c r="M29" s="29">
-        <v>14</v>
-      </c>
-      <c r="N29">
-        <f>M29/L29</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="5">
-        <v>6</v>
-      </c>
-      <c r="C30" s="6">
-        <v>12</v>
-      </c>
-      <c r="D30" s="7">
-        <f>C30/B30</f>
-        <v>2</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="5">
-        <v>4</v>
-      </c>
-      <c r="H30" s="30">
-        <v>5</v>
-      </c>
-      <c r="I30" s="7">
-        <f>H30/G30</f>
-        <v>1.25</v>
-      </c>
-      <c r="K30" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="28">
-        <v>2</v>
-      </c>
-      <c r="M30" s="29">
-        <v>14</v>
-      </c>
-      <c r="N30">
-        <f>M30/L30</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="5">
-        <v>3</v>
-      </c>
-      <c r="C31" s="6">
-        <v>5</v>
-      </c>
-      <c r="D31" s="7">
-        <f>C31/B31</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="F31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="5">
-        <v>3</v>
-      </c>
-      <c r="H31" s="30">
-        <v>3</v>
-      </c>
-      <c r="I31" s="7">
-        <f>H31/G31</f>
-        <v>1</v>
-      </c>
-      <c r="K31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L31" s="28">
-        <v>2</v>
-      </c>
-      <c r="M31" s="29">
-        <v>14</v>
-      </c>
-      <c r="N31">
-        <f>M31/L31</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="5">
-        <v>3</v>
-      </c>
-      <c r="C32" s="6">
-        <v>3</v>
-      </c>
-      <c r="D32" s="7">
-        <f>C32/B32</f>
-        <v>1</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="5">
-        <v>4</v>
-      </c>
-      <c r="H32" s="30">
-        <v>3</v>
-      </c>
-      <c r="I32" s="7">
-        <f>H32/G32</f>
-        <v>0.75</v>
-      </c>
-      <c r="K32" t="s">
-        <v>26</v>
-      </c>
-      <c r="L32" s="28">
-        <v>2</v>
-      </c>
-      <c r="M32" s="29">
-        <v>20</v>
-      </c>
-      <c r="N32">
-        <f>M32/L32</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="5">
-        <v>1</v>
-      </c>
-      <c r="C33" s="6">
-        <v>3</v>
-      </c>
-      <c r="D33" s="7">
-        <f>C33/B33</f>
-        <v>3</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G33" s="5">
-        <v>1</v>
-      </c>
-      <c r="H33" s="30">
-        <v>3</v>
-      </c>
-      <c r="I33" s="7">
-        <f>H33/G33</f>
-        <v>3</v>
-      </c>
-      <c r="K33" t="s">
-        <v>27</v>
-      </c>
-      <c r="L33" s="28">
-        <v>2</v>
-      </c>
-      <c r="M33" s="29">
-        <v>32</v>
-      </c>
-      <c r="N33">
-        <f>M33/L33</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="5">
-        <v>2</v>
-      </c>
-      <c r="C34" s="6">
-        <v>9</v>
-      </c>
-      <c r="D34" s="7">
-        <f>C34/B34</f>
-        <v>4.5</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="5">
-        <v>2</v>
-      </c>
-      <c r="H34" s="30">
-        <v>4</v>
-      </c>
-      <c r="I34" s="7">
-        <f>H34/G34</f>
-        <v>2</v>
-      </c>
-      <c r="K34" t="s">
-        <v>23</v>
-      </c>
-      <c r="L34" s="28">
-        <v>2</v>
-      </c>
-      <c r="M34" s="29">
-        <v>44</v>
-      </c>
-      <c r="N34">
-        <f>M34/L34</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="N38" s="11"/>
-    </row>
-    <row r="58" spans="14:14">
-      <c r="N58" s="16"/>
-    </row>
-    <row r="59" spans="14:14">
-      <c r="N59" s="16"/>
-    </row>
-    <row r="60" spans="14:14">
-      <c r="N60" s="16"/>
-    </row>
-    <row r="61" spans="14:14">
-      <c r="N61" s="16"/>
-    </row>
-    <row r="62" spans="14:14">
-      <c r="N62" s="16"/>
-    </row>
-    <row r="63" spans="14:14">
-      <c r="N63" s="16"/>
-    </row>
-    <row r="64" spans="14:14">
-      <c r="N64" s="16"/>
-    </row>
-    <row r="65" spans="13:14">
-      <c r="N65" s="16"/>
-    </row>
-    <row r="66" spans="13:14">
-      <c r="M66" s="16"/>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="O38" s="11"/>
+    </row>
+    <row r="58" spans="15:15">
+      <c r="O58" s="16"/>
+    </row>
+    <row r="59" spans="15:15">
+      <c r="O59" s="16"/>
+    </row>
+    <row r="60" spans="15:15">
+      <c r="O60" s="16"/>
+    </row>
+    <row r="61" spans="15:15">
+      <c r="O61" s="16"/>
+    </row>
+    <row r="62" spans="15:15">
+      <c r="O62" s="16"/>
+    </row>
+    <row r="63" spans="15:15">
+      <c r="O63" s="16"/>
+    </row>
+    <row r="64" spans="15:15">
+      <c r="O64" s="16"/>
+    </row>
+    <row r="65" spans="14:15">
+      <c r="O65" s="16"/>
+    </row>
+    <row r="66" spans="14:15">
       <c r="N66" s="16"/>
-    </row>
-    <row r="67" spans="13:14">
-      <c r="M67" s="4"/>
+      <c r="O66" s="16"/>
+    </row>
+    <row r="67" spans="14:15">
       <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A6:N34">
-    <sortCondition ref="N6:N34"/>
+  <sortState ref="B6:O34">
+    <sortCondition ref="E6:E34"/>
   </sortState>
   <mergeCells count="4">
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="B1:O2"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="61" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>